<commit_message>
db import & button dynamic & tutorial
</commit_message>
<xml_diff>
--- a/데이터베이스_내부.xlsx
+++ b/데이터베이스_내부.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390" tabRatio="697"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390" tabRatio="697" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="계정" sheetId="1" r:id="rId1"/>
-    <sheet name="스테이지 클리어 정보" sheetId="3" r:id="rId2"/>
-    <sheet name="멀티 플레이" sheetId="5" r:id="rId3"/>
+    <sheet name="스테이지 정보" sheetId="6" r:id="rId2"/>
+    <sheet name="스테이지 클리어 정보" sheetId="3" r:id="rId3"/>
+    <sheet name="멀티 플레이" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="72">
   <si>
     <t>계정</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -237,6 +238,82 @@
   </si>
   <si>
     <t>별 개수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스테이지 정보</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SINGLE_MAP_5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스테이지 번호(pri)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NUMBER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>최소</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int(4)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MIN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>중간</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>최대</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int(4)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MAX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(500)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MAP_INFO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map_size</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int(4)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MAP_SIZE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5+5-1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -593,8 +670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -733,6 +810,104 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F7"/>
   <sheetViews>
@@ -790,7 +965,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F8"/>
   <sheetViews>

</xml_diff>